<commit_message>
mustery shopping double check
</commit_message>
<xml_diff>
--- a/Tables_excel/Mystery_2022/Raw_data/FINAL_2DII All Countires 2022-2023.xlsx
+++ b/Tables_excel/Mystery_2022/Raw_data/FINAL_2DII All Countires 2022-2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnaKatherineRiveraMo\Documents\GitHub\Data.2DII\Tables_excel\Mystery_2022\Raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84ADABF-2AAD-4EC7-9CDB-C2501E82C31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90C5912-8A80-4741-B1A4-58445C6BE17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -4585,7 +4585,7 @@
   <dimension ref="A1:CK254"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="Q1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -59308,15 +59308,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E19E5E8875742644AB11D2685660DAC2" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7b3bacd36cf8428e29ded372b81b042a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2ddec4f4-1302-4af8-92c6-ad02e17aec3c" xmlns:ns3="603db874-dc9b-464f-ab52-27fac079c284" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c1a25e276ee3c2fbeec74227983efd8" ns2:_="" ns3:_="">
     <xsd:import namespace="2ddec4f4-1302-4af8-92c6-ad02e17aec3c"/>
@@ -59565,15 +59556,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31B06553-5CD4-49E5-A1FF-A8C962F5315B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53A92C94-A1BC-4EC7-84AD-5A465196C5F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -59590,4 +59582,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31B06553-5CD4-49E5-A1FF-A8C962F5315B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>